<commit_message>
cleaned up figure and table directory
</commit_message>
<xml_diff>
--- a/figures_tables/tables.xlsx
+++ b/figures_tables/tables.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheila/Documents/github/paper-d18o-phosphate-riparian/figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssaia/Documents/github/paper-d18o-phosphate-riparian/figures_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F611E3E-2737-424F-81F9-B32C9872E72A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22800" yWindow="480" windowWidth="14360" windowHeight="20880" activeTab="2" xr2:uid="{613A7F2E-40C4-AC4B-91A5-539A1962CDCE}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="27840" windowHeight="17500"/>
   </bookViews>
   <sheets>
     <sheet name="d18O-phos model" sheetId="1" r:id="rId1"/>
     <sheet name="Pi models" sheetId="2" r:id="rId2"/>
     <sheet name="Po models" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t>Model</t>
   </si>
@@ -261,12 +266,15 @@
   </si>
   <si>
     <t>HCl Extract</t>
+  </si>
+  <si>
+    <t>This tab was generated manually by Sheila Saia.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -334,7 +342,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -342,10 +350,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -768,11 +776,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BBF209-8FF2-004D-A472-44F7D7981EF0}">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,17 +902,22 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4940B48-DE34-C34F-8451-9676F5886F82}">
-  <dimension ref="A1:G36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,17 +1314,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF250BF-E030-9146-A537-7F0812F51CAD}">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1704,6 +1722,11 @@
         <v>70</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>